<commit_message>
Updated link in readme. Fixed typos
</commit_message>
<xml_diff>
--- a/Generic dependent dropdowns 2025.xlsx
+++ b/Generic dependent dropdowns 2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c4781e6f10de075/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devel\GitHub\dependent-dropdowns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="13_ncr:1_{3FC79A4F-F7B0-40B9-AB82-38BC5106D40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49C40D8F-4EEC-4902-954A-A75F6F0A4365}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17F5967-4722-4417-9A7B-C9259A47C44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="695" xr2:uid="{CFE9C8BB-2459-420C-9738-69DA0FE3A2B5}"/>
   </bookViews>
@@ -724,7 +724,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> Rename the columns as needed in Drop-Downs and Master Data. You may delete and add columns to accomodate your required number of levels.</a:t>
+            <a:t> Rename the columns as needed in Drop-Downs and Master Data. You may delete and add columns to accommodate your required number of levels.</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR">
             <a:effectLst/>
@@ -874,7 +874,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> A dynamic array formula builds a table with the list contents for each possible selection combinations in the Work tab. </a:t>
+            <a:t> A dynamic array formula builds a table with the list contents for each possible selection combination in the Work tab. </a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100">
             <a:solidFill>
@@ -1159,36 +1159,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>This file is available for download from https://github.com/tirlibibi17/dependent-dropdowns/tree/main</a:t>
+            <a:t>This file is available for download from https://github.com/tirlibibi17/dependent-dropdowns/blob/main/Generic%20dependent%20dropdowns%202025.xlsx</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR" sz="1100" b="0" i="0" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -1720,7 +1692,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>